<commit_message>
use row.WriteSlice to write head
</commit_message>
<xml_diff>
--- a/appinv/out/09102989061-4.xlsx
+++ b/appinv/out/09102989061-4.xlsx
@@ -679,7 +679,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -730,7 +730,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s"/>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -748,7 +748,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s"/>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -797,7 +797,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -848,7 +848,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s"/>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -897,7 +897,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -948,7 +948,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s"/>
-      <c r="B13" s="5">
+      <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -997,7 +997,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1048,7 +1048,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s"/>
-      <c r="B17" s="5">
+      <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1097,7 +1097,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1148,7 +1148,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s"/>
-      <c r="B21" s="5">
+      <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1197,7 +1197,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2">
+      <c r="A23">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1248,7 +1248,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s"/>
-      <c r="B25" s="5">
+      <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1297,7 +1297,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2">
+      <c r="A27">
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s"/>
-      <c r="B29" s="5">
+      <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -1366,7 +1366,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s"/>
-      <c r="B30" s="5">
+      <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1384,7 +1384,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s"/>
-      <c r="B31" s="5">
+      <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -1402,7 +1402,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s"/>
-      <c r="B32" s="5">
+      <c r="B32">
         <v>4</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -1451,7 +1451,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2">
+      <c r="A34">
         <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1502,7 +1502,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s"/>
-      <c r="B36" s="5">
+      <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -1520,7 +1520,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s"/>
-      <c r="B37" s="5">
+      <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1538,7 +1538,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s"/>
-      <c r="B38" s="5">
+      <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1587,7 +1587,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2">
+      <c r="A40">
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1638,7 +1638,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s"/>
-      <c r="B42" s="5">
+      <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -1656,7 +1656,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s"/>
-      <c r="B43" s="5">
+      <c r="B43">
         <v>2</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -1705,7 +1705,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2">
+      <c r="A45">
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1756,7 +1756,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s"/>
-      <c r="B47" s="5">
+      <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2">
+      <c r="A49">
         <v>11</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -1856,7 +1856,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s"/>
-      <c r="B51" s="5">
+      <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -1905,7 +1905,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2">
+      <c r="A53">
         <v>12</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1956,7 +1956,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s"/>
-      <c r="B55" s="5">
+      <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -1974,7 +1974,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s"/>
-      <c r="B56" s="5">
+      <c r="B56">
         <v>2</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2">
+      <c r="A58">
         <v>13</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -2074,7 +2074,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s"/>
-      <c r="B60" s="5">
+      <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
@@ -2092,7 +2092,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s"/>
-      <c r="B61" s="5">
+      <c r="B61">
         <v>2</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2">
+      <c r="A63">
         <v>14</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2192,7 +2192,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s"/>
-      <c r="B65" s="5">
+      <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2210,7 +2210,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s"/>
-      <c r="B66" s="5">
+      <c r="B66">
         <v>2</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2228,7 +2228,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s"/>
-      <c r="B67" s="5">
+      <c r="B67">
         <v>3</v>
       </c>
       <c r="C67" s="5" t="s">
@@ -2246,7 +2246,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s"/>
-      <c r="B68" s="5">
+      <c r="B68">
         <v>4</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -2264,7 +2264,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s"/>
-      <c r="B69" s="5">
+      <c r="B69">
         <v>5</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -2313,7 +2313,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2">
+      <c r="A71">
         <v>15</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -2364,7 +2364,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s"/>
-      <c r="B73" s="5">
+      <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" s="5" t="s">
@@ -2413,7 +2413,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2">
+      <c r="A75">
         <v>16</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -2464,7 +2464,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s"/>
-      <c r="B77" s="5">
+      <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" s="5" t="s">

</xml_diff>